<commit_message>
Added Json to Collapse list view
</commit_message>
<xml_diff>
--- a/Documentation/work-log.xlsx
+++ b/Documentation/work-log.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7650410903407856/Desktop/Taxii-Proxy/Documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\corte\Desktop\Taxii-Proxy-React\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="113" documentId="13_ncr:1_{6B1A99C6-E45B-4927-BC63-C83B0862564A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5BEFBD5A-2B8B-4827-BE22-978C4AEB26A6}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{200F3C13-2C17-4CA9-A540-6D61C45942FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" activeTab="1" xr2:uid="{29AACAA8-21F2-47DA-A7FC-DC118A90FAF2}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" activeTab="2" xr2:uid="{29AACAA8-21F2-47DA-A7FC-DC118A90FAF2}"/>
   </bookViews>
   <sheets>
     <sheet name="Progress Report 2" sheetId="1" r:id="rId1"/>
     <sheet name="Progress Report 3" sheetId="2" r:id="rId2"/>
+    <sheet name="Progress  Report 4" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="31">
   <si>
     <t>Time</t>
   </si>
@@ -262,6 +263,21 @@
         <scheme val="minor"/>
       </rPr>
       <t>Identified backend API requirements for passing information between Flask and React. Heavy compliation and validation will be done using python in Flask server while React frontend handles all visuals.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Dev Session: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Displayed STIX objects in visualizer</t>
     </r>
   </si>
 </sst>
@@ -665,6 +681,9 @@
     <xf numFmtId="20" fontId="2" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="20" fontId="2" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -673,9 +692,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1017,24 +1033,24 @@
       <selection sqref="A1:F35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="36.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" customWidth="1"/>
+    <col min="1" max="1" width="36.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="34"/>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="35"/>
+    </row>
+    <row r="2" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
@@ -1054,7 +1070,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="15" t="s">
         <v>10</v>
       </c>
@@ -1073,7 +1089,7 @@
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="22" t="s">
         <v>13</v>
       </c>
@@ -1092,7 +1108,7 @@
       </c>
       <c r="F4" s="17"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="22" t="s">
         <v>12</v>
       </c>
@@ -1111,7 +1127,7 @@
       </c>
       <c r="F5" s="17"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="22" t="s">
         <v>11</v>
       </c>
@@ -1130,7 +1146,7 @@
       </c>
       <c r="F6" s="17"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="16" t="s">
         <v>9</v>
       </c>
@@ -1149,7 +1165,7 @@
       </c>
       <c r="F7" s="17"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="16" t="s">
         <v>8</v>
       </c>
@@ -1168,7 +1184,7 @@
       </c>
       <c r="F8" s="17"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="16" t="s">
         <v>21</v>
       </c>
@@ -1187,7 +1203,7 @@
       </c>
       <c r="F9" s="17"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="16" t="s">
         <v>14</v>
       </c>
@@ -1206,7 +1222,7 @@
       </c>
       <c r="F10" s="17"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="16" t="s">
         <v>14</v>
       </c>
@@ -1225,7 +1241,7 @@
       </c>
       <c r="F11" s="17"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="2" t="s">
         <v>7</v>
       </c>
@@ -1244,7 +1260,7 @@
       </c>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="2" t="s">
         <v>16</v>
       </c>
@@ -1263,7 +1279,7 @@
       </c>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="2" t="s">
         <v>17</v>
       </c>
@@ -1282,7 +1298,7 @@
       </c>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="2" t="s">
         <v>18</v>
       </c>
@@ -1301,7 +1317,7 @@
       </c>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="2" t="s">
         <v>18</v>
       </c>
@@ -1320,7 +1336,7 @@
       </c>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="2" t="s">
         <v>19</v>
       </c>
@@ -1339,7 +1355,7 @@
       </c>
       <c r="F17" s="4"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="2" t="s">
         <v>20</v>
       </c>
@@ -1358,7 +1374,7 @@
       </c>
       <c r="F18" s="4"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="2"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -1369,7 +1385,7 @@
       </c>
       <c r="F19" s="4"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" s="2"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -1380,7 +1396,7 @@
       </c>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" s="2"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -1391,7 +1407,7 @@
       </c>
       <c r="F21" s="4"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" s="2"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -1402,7 +1418,7 @@
       </c>
       <c r="F22" s="4"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" s="2"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -1413,7 +1429,7 @@
       </c>
       <c r="F23" s="4"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" s="2"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -1424,7 +1440,7 @@
       </c>
       <c r="F24" s="4"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" s="2"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -1435,7 +1451,7 @@
       </c>
       <c r="F25" s="4"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" s="2"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -1446,7 +1462,7 @@
       </c>
       <c r="F26" s="4"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" s="2"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -1457,7 +1473,7 @@
       </c>
       <c r="F27" s="4"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" s="2"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -1468,7 +1484,7 @@
       </c>
       <c r="F28" s="4"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" s="2"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -1479,7 +1495,7 @@
       </c>
       <c r="F29" s="4"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" s="2"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -1490,7 +1506,7 @@
       </c>
       <c r="F30" s="4"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" s="2"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -1501,7 +1517,7 @@
       </c>
       <c r="F31" s="4"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" s="2"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -1512,7 +1528,7 @@
       </c>
       <c r="F32" s="4"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33" s="2"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -1523,7 +1539,7 @@
       </c>
       <c r="F33" s="4"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34" s="2"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -1534,7 +1550,7 @@
       </c>
       <c r="F34" s="4"/>
     </row>
-    <row r="35" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A35" s="5"/>
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
@@ -1547,7 +1563,7 @@
       </c>
       <c r="F35" s="7"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="E36" s="24"/>
     </row>
   </sheetData>
@@ -1562,27 +1578,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{225D9EEB-461F-4A79-AC4A-E91E9ECD959A}">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F37" sqref="A1:F37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="36.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="34"/>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="35"/>
+    </row>
+    <row r="2" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
@@ -1602,7 +1618,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="57" x14ac:dyDescent="0.45">
       <c r="A3" s="31" t="s">
         <v>22</v>
       </c>
@@ -1621,7 +1637,7 @@
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A4" s="27" t="s">
         <v>27</v>
       </c>
@@ -1640,7 +1656,7 @@
       </c>
       <c r="F4" s="17"/>
     </row>
-    <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="57" x14ac:dyDescent="0.45">
       <c r="A5" s="27" t="s">
         <v>26</v>
       </c>
@@ -1659,8 +1675,8 @@
       </c>
       <c r="F5" s="17"/>
     </row>
-    <row r="6" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A6" s="35" t="s">
+    <row r="6" spans="1:6" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="A6" s="32" t="s">
         <v>29</v>
       </c>
       <c r="B6" s="18">
@@ -1678,7 +1694,7 @@
       </c>
       <c r="F6" s="17"/>
     </row>
-    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A7" s="27" t="s">
         <v>28</v>
       </c>
@@ -1697,8 +1713,8 @@
       </c>
       <c r="F7" s="17"/>
     </row>
-    <row r="8" spans="1:6" ht="165" x14ac:dyDescent="0.25">
-      <c r="A8" s="35" t="s">
+    <row r="8" spans="1:6" ht="142.5" x14ac:dyDescent="0.45">
+      <c r="A8" s="32" t="s">
         <v>25</v>
       </c>
       <c r="B8" s="18">
@@ -1716,7 +1732,7 @@
       </c>
       <c r="F8" s="17"/>
     </row>
-    <row r="9" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A9" s="28" t="s">
         <v>24</v>
       </c>
@@ -1735,7 +1751,7 @@
       </c>
       <c r="F9" s="17"/>
     </row>
-    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A10" s="28" t="s">
         <v>23</v>
       </c>
@@ -1754,7 +1770,7 @@
       </c>
       <c r="F10" s="17"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="28"/>
       <c r="B11" s="18"/>
       <c r="C11" s="19"/>
@@ -1765,7 +1781,7 @@
       </c>
       <c r="F11" s="17"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="28"/>
       <c r="B12" s="18"/>
       <c r="C12" s="19"/>
@@ -1776,7 +1792,7 @@
       </c>
       <c r="F12" s="17"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="28"/>
       <c r="B13" s="18"/>
       <c r="C13" s="19"/>
@@ -1787,7 +1803,7 @@
       </c>
       <c r="F13" s="17"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="29"/>
       <c r="B14" s="12"/>
       <c r="C14" s="13"/>
@@ -1798,7 +1814,7 @@
       </c>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="29"/>
       <c r="B15" s="12"/>
       <c r="C15" s="13"/>
@@ -1809,7 +1825,7 @@
       </c>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="29"/>
       <c r="B16" s="12"/>
       <c r="C16" s="13"/>
@@ -1820,7 +1836,7 @@
       </c>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="29"/>
       <c r="B17" s="12"/>
       <c r="C17" s="13"/>
@@ -1831,7 +1847,7 @@
       </c>
       <c r="F17" s="4"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="29"/>
       <c r="B18" s="12"/>
       <c r="C18" s="13"/>
@@ -1842,7 +1858,7 @@
       </c>
       <c r="F18" s="4"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="29"/>
       <c r="B19" s="12"/>
       <c r="C19" s="13"/>
@@ -1853,7 +1869,7 @@
       </c>
       <c r="F19" s="4"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" s="29"/>
       <c r="B20" s="12"/>
       <c r="C20" s="13"/>
@@ -1864,7 +1880,7 @@
       </c>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" s="29"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -1875,7 +1891,7 @@
       </c>
       <c r="F21" s="4"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" s="29"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -1886,7 +1902,7 @@
       </c>
       <c r="F22" s="4"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" s="29"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -1897,7 +1913,7 @@
       </c>
       <c r="F23" s="4"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" s="29"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -1908,7 +1924,7 @@
       </c>
       <c r="F24" s="4"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" s="29"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -1919,7 +1935,7 @@
       </c>
       <c r="F25" s="4"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" s="29"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -1930,7 +1946,7 @@
       </c>
       <c r="F26" s="4"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" s="29"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -1941,7 +1957,7 @@
       </c>
       <c r="F27" s="4"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" s="29"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -1952,7 +1968,7 @@
       </c>
       <c r="F28" s="4"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" s="29"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -1963,7 +1979,7 @@
       </c>
       <c r="F29" s="4"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" s="29"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -1974,7 +1990,7 @@
       </c>
       <c r="F30" s="4"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" s="29"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -1985,7 +2001,7 @@
       </c>
       <c r="F31" s="4"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" s="29"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -1996,7 +2012,7 @@
       </c>
       <c r="F32" s="4"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33" s="29"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -2007,7 +2023,7 @@
       </c>
       <c r="F33" s="4"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34" s="29"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -2018,7 +2034,7 @@
       </c>
       <c r="F34" s="4"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35" s="29"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -2029,7 +2045,7 @@
       </c>
       <c r="F35" s="4"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" s="29"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -2040,7 +2056,7 @@
       </c>
       <c r="F36" s="4"/>
     </row>
-    <row r="37" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A37" s="30"/>
       <c r="B37" s="6"/>
       <c r="C37" s="6"/>
@@ -2059,4 +2075,452 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E2B1528-2155-494F-8891-045CE16F69FD}">
+  <dimension ref="A1:F37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="27" customWidth="1"/>
+    <col min="2" max="2" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="35"/>
+    </row>
+    <row r="2" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A3" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="20">
+        <v>45341</v>
+      </c>
+      <c r="C3" s="21">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="D3" s="21">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="E3" s="15">
+        <f t="shared" ref="E3:E36" si="0">D3-C3</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" s="27"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F4" s="17"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" s="27"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F5" s="17"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" s="32"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F6" s="17"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" s="27"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F7" s="17"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8" s="32"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F8" s="17"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9" s="28"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F9" s="17"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10" s="28"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F10" s="17"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11" s="28"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F11" s="17"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12" s="28"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F12" s="17"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A13" s="28"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F13" s="17"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A14" s="29"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F14" s="4"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A15" s="29"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F15" s="4"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A16" s="29"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F16" s="4"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A17" s="29"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F17" s="4"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A18" s="29"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F18" s="4"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A19" s="29"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F19" s="4"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A20" s="29"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F20" s="4"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A21" s="29"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F21" s="4"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A22" s="29"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F22" s="4"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A23" s="29"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F23" s="4"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A24" s="29"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F24" s="4"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A25" s="29"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F25" s="4"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A26" s="29"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F26" s="4"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A27" s="29"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F27" s="4"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A28" s="29"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F28" s="4"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A29" s="29"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F29" s="4"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A30" s="29"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F30" s="4"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A31" s="29"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F31" s="4"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A32" s="29"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F32" s="4"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A33" s="29"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F33" s="4"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A34" s="29"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F34" s="4"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A35" s="29"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F35" s="4"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A36" s="29"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F36" s="4"/>
+    </row>
+    <row r="37" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A37" s="30"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="E37" s="26">
+        <f>SUM(E3:E36)</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="F37" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Broke Network Graph added
</commit_message>
<xml_diff>
--- a/Documentation/work-log.xlsx
+++ b/Documentation/work-log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7650410903407856/Desktop/Taxii-Proxy/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="113" documentId="13_ncr:1_{6B1A99C6-E45B-4927-BC63-C83B0862564A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5BEFBD5A-2B8B-4827-BE22-978C4AEB26A6}"/>
+  <xr:revisionPtr revIDLastSave="116" documentId="13_ncr:1_{6B1A99C6-E45B-4927-BC63-C83B0862564A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A9E8DAE2-F6E4-4E8E-B946-F1A87FBAFB69}"/>
   <bookViews>
     <workbookView xWindow="4770" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{29AACAA8-21F2-47DA-A7FC-DC118A90FAF2}"/>
   </bookViews>
@@ -17,7 +17,6 @@
     <sheet name="Progress Report 3" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
   <si>
     <t>Time</t>
   </si>
@@ -264,6 +263,9 @@
       </rPr>
       <t>Identified backend API requirements for passing information between Flask and React. Heavy compliation and validation will be done using python in Flask server while React frontend handles all visuals.</t>
     </r>
+  </si>
+  <si>
+    <t>Dev Session: Worked on Implementing Visualizer page for TAXII Proxy</t>
   </si>
 </sst>
 </file>
@@ -619,7 +621,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -677,6 +679,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1567,8 +1572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{225D9EEB-461F-4A79-AC4A-E91E9ECD959A}">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1759,14 +1764,20 @@
       </c>
       <c r="F10" s="17"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="28"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="19"/>
+    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="18">
+        <v>45347</v>
+      </c>
+      <c r="C11" s="19">
+        <v>0.625</v>
+      </c>
       <c r="D11" s="19"/>
       <c r="E11" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-0.625</v>
       </c>
       <c r="F11" s="17"/>
     </row>
@@ -2054,7 +2065,7 @@
       </c>
       <c r="E37" s="26">
         <f>SUM(E3:E36)</f>
-        <v>1.1666666666666667</v>
+        <v>0.54166666666666674</v>
       </c>
       <c r="F37" s="7"/>
     </row>

</xml_diff>

<commit_message>
added arrow heads to links
</commit_message>
<xml_diff>
--- a/Documentation/work-log.xlsx
+++ b/Documentation/work-log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7650410903407856/Desktop/Taxii-Proxy/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="130" documentId="13_ncr:1_{6B1A99C6-E45B-4927-BC63-C83B0862564A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{256C2E83-2C21-4FE1-87D7-E37725111527}"/>
+  <xr:revisionPtr revIDLastSave="135" documentId="13_ncr:1_{6B1A99C6-E45B-4927-BC63-C83B0862564A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8D979D83-39EB-43D5-B0B6-E805C2B43EF9}"/>
   <bookViews>
     <workbookView xWindow="4995" yWindow="-13470" windowWidth="28800" windowHeight="11295" activeTab="2" xr2:uid="{29AACAA8-21F2-47DA-A7FC-DC118A90FAF2}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="33">
   <si>
     <t>Time</t>
   </si>
@@ -281,6 +281,29 @@
         <scheme val="minor"/>
       </rPr>
       <t>Developing STIX bundle parsing into network graph nodes and links</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Visualizer:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Improve node information displayed</t>
     </r>
   </si>
 </sst>
@@ -2098,7 +2121,7 @@
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2156,13 +2179,21 @@
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="27"/>
-      <c r="B4" s="18"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
+      <c r="A4" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="18">
+        <v>45358</v>
+      </c>
+      <c r="C4" s="19">
+        <v>0.90972222222222221</v>
+      </c>
+      <c r="D4" s="19">
+        <v>0.95833333333333337</v>
+      </c>
       <c r="E4" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.861111111111116E-2</v>
       </c>
       <c r="F4" s="17"/>
     </row>
@@ -2527,7 +2558,7 @@
       </c>
       <c r="E37" s="26">
         <f>SUM(E3:E36)</f>
-        <v>9.722222222222221E-2</v>
+        <v>0.14583333333333337</v>
       </c>
       <c r="F37" s="7"/>
     </row>

</xml_diff>

<commit_message>
Created API call for Validation of bundles
</commit_message>
<xml_diff>
--- a/Documentation/work-log.xlsx
+++ b/Documentation/work-log.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7650410903407856/Desktop/Taxii-Proxy/Documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\corte\Desktop\Taxii-Proxy-React\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{7B6702CC-EE36-4191-9492-BDB01E6BCDDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{790F5388-98EA-4631-9E84-8D2347FC0DC7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{341A3148-6363-494D-ABFD-1E4CCF267BD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4995" yWindow="-13470" windowWidth="28800" windowHeight="11295" activeTab="3" xr2:uid="{29AACAA8-21F2-47DA-A7FC-DC118A90FAF2}"/>
+    <workbookView xWindow="3308" yWindow="3308" windowWidth="16875" windowHeight="10432" activeTab="3" xr2:uid="{29AACAA8-21F2-47DA-A7FC-DC118A90FAF2}"/>
   </bookViews>
   <sheets>
     <sheet name="Progress Report 2" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,6 @@
     <sheet name="Report 6" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="42">
   <si>
     <t>Time</t>
   </si>
@@ -441,6 +440,75 @@
         <scheme val="minor"/>
       </rPr>
       <t>Schema Development</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Dev: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Added the ability to select a schema based on a list that is pulled from the API backend</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Dev: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Add STIX 2.1 Validation</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Dev</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Add STIX 2.1 Validation</t>
     </r>
   </si>
 </sst>
@@ -874,10 +942,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1203,14 +1267,14 @@
       <selection sqref="A1:F35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="36.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" customWidth="1"/>
+    <col min="1" max="1" width="36.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="34" t="s">
         <v>6</v>
       </c>
@@ -1220,7 +1284,7 @@
       <c r="E1" s="35"/>
       <c r="F1" s="36"/>
     </row>
-    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
@@ -1240,7 +1304,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="15" t="s">
         <v>10</v>
       </c>
@@ -1259,7 +1323,7 @@
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="22" t="s">
         <v>13</v>
       </c>
@@ -1278,7 +1342,7 @@
       </c>
       <c r="F4" s="17"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="22" t="s">
         <v>12</v>
       </c>
@@ -1297,7 +1361,7 @@
       </c>
       <c r="F5" s="17"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="22" t="s">
         <v>11</v>
       </c>
@@ -1316,7 +1380,7 @@
       </c>
       <c r="F6" s="17"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="16" t="s">
         <v>9</v>
       </c>
@@ -1335,7 +1399,7 @@
       </c>
       <c r="F7" s="17"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="16" t="s">
         <v>8</v>
       </c>
@@ -1354,7 +1418,7 @@
       </c>
       <c r="F8" s="17"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="16" t="s">
         <v>21</v>
       </c>
@@ -1373,7 +1437,7 @@
       </c>
       <c r="F9" s="17"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="16" t="s">
         <v>14</v>
       </c>
@@ -1392,7 +1456,7 @@
       </c>
       <c r="F10" s="17"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="16" t="s">
         <v>14</v>
       </c>
@@ -1411,7 +1475,7 @@
       </c>
       <c r="F11" s="17"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="2" t="s">
         <v>7</v>
       </c>
@@ -1430,7 +1494,7 @@
       </c>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="2" t="s">
         <v>16</v>
       </c>
@@ -1449,7 +1513,7 @@
       </c>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="2" t="s">
         <v>17</v>
       </c>
@@ -1468,7 +1532,7 @@
       </c>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="2" t="s">
         <v>18</v>
       </c>
@@ -1487,7 +1551,7 @@
       </c>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="2" t="s">
         <v>18</v>
       </c>
@@ -1506,7 +1570,7 @@
       </c>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="2" t="s">
         <v>19</v>
       </c>
@@ -1525,7 +1589,7 @@
       </c>
       <c r="F17" s="4"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="2" t="s">
         <v>20</v>
       </c>
@@ -1544,7 +1608,7 @@
       </c>
       <c r="F18" s="4"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="2"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -1555,7 +1619,7 @@
       </c>
       <c r="F19" s="4"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" s="2"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -1566,7 +1630,7 @@
       </c>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" s="2"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -1577,7 +1641,7 @@
       </c>
       <c r="F21" s="4"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" s="2"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -1588,7 +1652,7 @@
       </c>
       <c r="F22" s="4"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" s="2"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -1599,7 +1663,7 @@
       </c>
       <c r="F23" s="4"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" s="2"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -1610,7 +1674,7 @@
       </c>
       <c r="F24" s="4"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" s="2"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -1621,7 +1685,7 @@
       </c>
       <c r="F25" s="4"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" s="2"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -1632,7 +1696,7 @@
       </c>
       <c r="F26" s="4"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" s="2"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -1643,7 +1707,7 @@
       </c>
       <c r="F27" s="4"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" s="2"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -1654,7 +1718,7 @@
       </c>
       <c r="F28" s="4"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" s="2"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -1665,7 +1729,7 @@
       </c>
       <c r="F29" s="4"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" s="2"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -1676,7 +1740,7 @@
       </c>
       <c r="F30" s="4"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" s="2"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -1687,7 +1751,7 @@
       </c>
       <c r="F31" s="4"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" s="2"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -1698,7 +1762,7 @@
       </c>
       <c r="F32" s="4"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33" s="2"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -1709,7 +1773,7 @@
       </c>
       <c r="F33" s="4"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34" s="2"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -1720,7 +1784,7 @@
       </c>
       <c r="F34" s="4"/>
     </row>
-    <row r="35" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A35" s="5"/>
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
@@ -1733,7 +1797,7 @@
       </c>
       <c r="F35" s="7"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="E36" s="24"/>
     </row>
   </sheetData>
@@ -1752,13 +1816,13 @@
       <selection sqref="A1:F37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="36.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="34" t="s">
         <v>6</v>
       </c>
@@ -1768,7 +1832,7 @@
       <c r="E1" s="35"/>
       <c r="F1" s="36"/>
     </row>
-    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
@@ -1788,7 +1852,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="57" x14ac:dyDescent="0.45">
       <c r="A3" s="31" t="s">
         <v>22</v>
       </c>
@@ -1807,7 +1871,7 @@
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A4" s="27" t="s">
         <v>27</v>
       </c>
@@ -1826,7 +1890,7 @@
       </c>
       <c r="F4" s="17"/>
     </row>
-    <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="57" x14ac:dyDescent="0.45">
       <c r="A5" s="27" t="s">
         <v>26</v>
       </c>
@@ -1845,7 +1909,7 @@
       </c>
       <c r="F5" s="17"/>
     </row>
-    <row r="6" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A6" s="32" t="s">
         <v>29</v>
       </c>
@@ -1864,7 +1928,7 @@
       </c>
       <c r="F6" s="17"/>
     </row>
-    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A7" s="27" t="s">
         <v>28</v>
       </c>
@@ -1883,7 +1947,7 @@
       </c>
       <c r="F7" s="17"/>
     </row>
-    <row r="8" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="142.5" x14ac:dyDescent="0.45">
       <c r="A8" s="32" t="s">
         <v>25</v>
       </c>
@@ -1902,7 +1966,7 @@
       </c>
       <c r="F8" s="17"/>
     </row>
-    <row r="9" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A9" s="28" t="s">
         <v>24</v>
       </c>
@@ -1921,7 +1985,7 @@
       </c>
       <c r="F9" s="17"/>
     </row>
-    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A10" s="28" t="s">
         <v>23</v>
       </c>
@@ -1940,7 +2004,7 @@
       </c>
       <c r="F10" s="17"/>
     </row>
-    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A11" s="33" t="s">
         <v>30</v>
       </c>
@@ -1957,7 +2021,7 @@
       </c>
       <c r="F11" s="17"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="28"/>
       <c r="B12" s="18"/>
       <c r="C12" s="19"/>
@@ -1968,7 +2032,7 @@
       </c>
       <c r="F12" s="17"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="28"/>
       <c r="B13" s="18"/>
       <c r="C13" s="19"/>
@@ -1979,7 +2043,7 @@
       </c>
       <c r="F13" s="17"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="29"/>
       <c r="B14" s="12"/>
       <c r="C14" s="13"/>
@@ -1990,7 +2054,7 @@
       </c>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="29"/>
       <c r="B15" s="12"/>
       <c r="C15" s="13"/>
@@ -2001,7 +2065,7 @@
       </c>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="29"/>
       <c r="B16" s="12"/>
       <c r="C16" s="13"/>
@@ -2012,7 +2076,7 @@
       </c>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="29"/>
       <c r="B17" s="12"/>
       <c r="C17" s="13"/>
@@ -2023,7 +2087,7 @@
       </c>
       <c r="F17" s="4"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="29"/>
       <c r="B18" s="12"/>
       <c r="C18" s="13"/>
@@ -2034,7 +2098,7 @@
       </c>
       <c r="F18" s="4"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="29"/>
       <c r="B19" s="12"/>
       <c r="C19" s="13"/>
@@ -2045,7 +2109,7 @@
       </c>
       <c r="F19" s="4"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" s="29"/>
       <c r="B20" s="12"/>
       <c r="C20" s="13"/>
@@ -2056,7 +2120,7 @@
       </c>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" s="29"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -2067,7 +2131,7 @@
       </c>
       <c r="F21" s="4"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" s="29"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -2078,7 +2142,7 @@
       </c>
       <c r="F22" s="4"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" s="29"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -2089,7 +2153,7 @@
       </c>
       <c r="F23" s="4"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" s="29"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -2100,7 +2164,7 @@
       </c>
       <c r="F24" s="4"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" s="29"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -2111,7 +2175,7 @@
       </c>
       <c r="F25" s="4"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" s="29"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -2122,7 +2186,7 @@
       </c>
       <c r="F26" s="4"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" s="29"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -2133,7 +2197,7 @@
       </c>
       <c r="F27" s="4"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" s="29"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -2144,7 +2208,7 @@
       </c>
       <c r="F28" s="4"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" s="29"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -2155,7 +2219,7 @@
       </c>
       <c r="F29" s="4"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" s="29"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -2166,7 +2230,7 @@
       </c>
       <c r="F30" s="4"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" s="29"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -2177,7 +2241,7 @@
       </c>
       <c r="F31" s="4"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" s="29"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -2188,7 +2252,7 @@
       </c>
       <c r="F32" s="4"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33" s="29"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -2199,7 +2263,7 @@
       </c>
       <c r="F33" s="4"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34" s="29"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -2210,7 +2274,7 @@
       </c>
       <c r="F34" s="4"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35" s="29"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -2221,7 +2285,7 @@
       </c>
       <c r="F35" s="4"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" s="29"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -2232,7 +2296,7 @@
       </c>
       <c r="F36" s="4"/>
     </row>
-    <row r="37" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A37" s="30"/>
       <c r="B37" s="6"/>
       <c r="C37" s="6"/>
@@ -2261,13 +2325,13 @@
       <selection sqref="A1:F37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="49" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="34" t="s">
         <v>6</v>
       </c>
@@ -2277,7 +2341,7 @@
       <c r="E1" s="35"/>
       <c r="F1" s="36"/>
     </row>
-    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
@@ -2297,7 +2361,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A3" s="31" t="s">
         <v>31</v>
       </c>
@@ -2316,7 +2380,7 @@
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="27" t="s">
         <v>32</v>
       </c>
@@ -2335,7 +2399,7 @@
       </c>
       <c r="F4" s="17"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="27" t="s">
         <v>32</v>
       </c>
@@ -2354,7 +2418,7 @@
       </c>
       <c r="F5" s="17"/>
     </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="27" t="s">
         <v>33</v>
       </c>
@@ -2373,7 +2437,7 @@
       </c>
       <c r="F6" s="17"/>
     </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="27" t="s">
         <v>33</v>
       </c>
@@ -2392,7 +2456,7 @@
       </c>
       <c r="F7" s="17"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="32" t="s">
         <v>34</v>
       </c>
@@ -2411,7 +2475,7 @@
       </c>
       <c r="F8" s="17"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="28" t="s">
         <v>35</v>
       </c>
@@ -2430,7 +2494,7 @@
       </c>
       <c r="F9" s="17"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="28" t="s">
         <v>36</v>
       </c>
@@ -2449,7 +2513,7 @@
       </c>
       <c r="F10" s="17"/>
     </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A11" s="33" t="s">
         <v>37</v>
       </c>
@@ -2468,7 +2532,7 @@
       </c>
       <c r="F11" s="17"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="28"/>
       <c r="B12" s="18"/>
       <c r="C12" s="19"/>
@@ -2479,7 +2543,7 @@
       </c>
       <c r="F12" s="17"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="28"/>
       <c r="B13" s="18"/>
       <c r="C13" s="19"/>
@@ -2490,7 +2554,7 @@
       </c>
       <c r="F13" s="17"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="29"/>
       <c r="B14" s="12"/>
       <c r="C14" s="13"/>
@@ -2501,7 +2565,7 @@
       </c>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="29"/>
       <c r="B15" s="12"/>
       <c r="C15" s="13"/>
@@ -2512,7 +2576,7 @@
       </c>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="29"/>
       <c r="B16" s="12"/>
       <c r="C16" s="13"/>
@@ -2523,7 +2587,7 @@
       </c>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="29"/>
       <c r="B17" s="12"/>
       <c r="C17" s="13"/>
@@ -2534,7 +2598,7 @@
       </c>
       <c r="F17" s="4"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="29"/>
       <c r="B18" s="12"/>
       <c r="C18" s="13"/>
@@ -2545,7 +2609,7 @@
       </c>
       <c r="F18" s="4"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="29"/>
       <c r="B19" s="12"/>
       <c r="C19" s="13"/>
@@ -2556,7 +2620,7 @@
       </c>
       <c r="F19" s="4"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" s="29"/>
       <c r="B20" s="12"/>
       <c r="C20" s="13"/>
@@ -2567,7 +2631,7 @@
       </c>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" s="29"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -2578,7 +2642,7 @@
       </c>
       <c r="F21" s="4"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" s="29"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -2589,7 +2653,7 @@
       </c>
       <c r="F22" s="4"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" s="29"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -2600,7 +2664,7 @@
       </c>
       <c r="F23" s="4"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" s="29"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -2611,7 +2675,7 @@
       </c>
       <c r="F24" s="4"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" s="29"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -2622,7 +2686,7 @@
       </c>
       <c r="F25" s="4"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" s="29"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -2633,7 +2697,7 @@
       </c>
       <c r="F26" s="4"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" s="29"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -2644,7 +2708,7 @@
       </c>
       <c r="F27" s="4"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" s="29"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -2655,7 +2719,7 @@
       </c>
       <c r="F28" s="4"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" s="29"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -2666,7 +2730,7 @@
       </c>
       <c r="F29" s="4"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" s="29"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -2677,7 +2741,7 @@
       </c>
       <c r="F30" s="4"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" s="29"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -2688,7 +2752,7 @@
       </c>
       <c r="F31" s="4"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" s="29"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -2699,7 +2763,7 @@
       </c>
       <c r="F32" s="4"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33" s="29"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -2710,7 +2774,7 @@
       </c>
       <c r="F33" s="4"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34" s="29"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -2721,7 +2785,7 @@
       </c>
       <c r="F34" s="4"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35" s="29"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -2732,7 +2796,7 @@
       </c>
       <c r="F35" s="4"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" s="29"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -2743,7 +2807,7 @@
       </c>
       <c r="F36" s="4"/>
     </row>
-    <row r="37" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A37" s="30"/>
       <c r="B37" s="6"/>
       <c r="C37" s="6"/>
@@ -2769,16 +2833,16 @@
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="67.28515625" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="67.265625" customWidth="1"/>
+    <col min="2" max="2" width="9.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="34" t="s">
         <v>6</v>
       </c>
@@ -2788,7 +2852,7 @@
       <c r="E1" s="35"/>
       <c r="F1" s="36"/>
     </row>
-    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
@@ -2808,7 +2872,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="31" t="s">
         <v>38</v>
       </c>
@@ -2827,40 +2891,64 @@
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="27"/>
-      <c r="B4" s="18"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
+    <row r="4" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A4" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="18">
+        <v>45008</v>
+      </c>
+      <c r="C4" s="19">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D4" s="19">
+        <v>0.83333333333333337</v>
+      </c>
       <c r="E4" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.16666666666666674</v>
       </c>
       <c r="F4" s="17"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="27"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="18">
+        <v>45009</v>
+      </c>
+      <c r="C5" s="19">
+        <v>0.4375</v>
+      </c>
+      <c r="D5" s="19">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="E5" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.14583333333333337</v>
       </c>
       <c r="F5" s="17"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="27"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="18">
+        <v>45010</v>
+      </c>
+      <c r="C6" s="19">
+        <v>0.89166666666666672</v>
+      </c>
+      <c r="D6" s="19">
+        <v>0.95833333333333337</v>
+      </c>
       <c r="E6" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.6666666666666652E-2</v>
       </c>
       <c r="F6" s="17"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="27"/>
       <c r="B7" s="18"/>
       <c r="C7" s="19"/>
@@ -2871,7 +2959,7 @@
       </c>
       <c r="F7" s="17"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="32"/>
       <c r="B8" s="18"/>
       <c r="C8" s="19"/>
@@ -2882,7 +2970,7 @@
       </c>
       <c r="F8" s="17"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="28"/>
       <c r="B9" s="18"/>
       <c r="C9" s="19"/>
@@ -2893,7 +2981,7 @@
       </c>
       <c r="F9" s="17"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="28"/>
       <c r="B10" s="18"/>
       <c r="C10" s="19"/>
@@ -2904,7 +2992,7 @@
       </c>
       <c r="F10" s="17"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="33"/>
       <c r="B11" s="18"/>
       <c r="C11" s="19"/>
@@ -2915,7 +3003,7 @@
       </c>
       <c r="F11" s="17"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="28"/>
       <c r="B12" s="18"/>
       <c r="C12" s="19"/>
@@ -2926,7 +3014,7 @@
       </c>
       <c r="F12" s="17"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="28"/>
       <c r="B13" s="18"/>
       <c r="C13" s="19"/>
@@ -2937,7 +3025,7 @@
       </c>
       <c r="F13" s="17"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="29"/>
       <c r="B14" s="12"/>
       <c r="C14" s="13"/>
@@ -2948,7 +3036,7 @@
       </c>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="29"/>
       <c r="B15" s="12"/>
       <c r="C15" s="13"/>
@@ -2959,7 +3047,7 @@
       </c>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="29"/>
       <c r="B16" s="12"/>
       <c r="C16" s="13"/>
@@ -2970,7 +3058,7 @@
       </c>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="29"/>
       <c r="B17" s="12"/>
       <c r="C17" s="13"/>
@@ -2981,7 +3069,7 @@
       </c>
       <c r="F17" s="4"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="29"/>
       <c r="B18" s="12"/>
       <c r="C18" s="13"/>
@@ -2992,7 +3080,7 @@
       </c>
       <c r="F18" s="4"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="29"/>
       <c r="B19" s="12"/>
       <c r="C19" s="13"/>
@@ -3003,7 +3091,7 @@
       </c>
       <c r="F19" s="4"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" s="29"/>
       <c r="B20" s="12"/>
       <c r="C20" s="13"/>
@@ -3014,7 +3102,7 @@
       </c>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" s="29"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -3025,7 +3113,7 @@
       </c>
       <c r="F21" s="4"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" s="29"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -3036,7 +3124,7 @@
       </c>
       <c r="F22" s="4"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" s="29"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -3047,7 +3135,7 @@
       </c>
       <c r="F23" s="4"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" s="29"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -3058,7 +3146,7 @@
       </c>
       <c r="F24" s="4"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" s="29"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -3069,7 +3157,7 @@
       </c>
       <c r="F25" s="4"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" s="29"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -3080,7 +3168,7 @@
       </c>
       <c r="F26" s="4"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" s="29"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -3091,7 +3179,7 @@
       </c>
       <c r="F27" s="4"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" s="29"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -3102,7 +3190,7 @@
       </c>
       <c r="F28" s="4"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" s="29"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -3113,7 +3201,7 @@
       </c>
       <c r="F29" s="4"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" s="29"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -3124,7 +3212,7 @@
       </c>
       <c r="F30" s="4"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" s="29"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -3135,7 +3223,7 @@
       </c>
       <c r="F31" s="4"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" s="29"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -3146,7 +3234,7 @@
       </c>
       <c r="F32" s="4"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33" s="29"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -3157,7 +3245,7 @@
       </c>
       <c r="F33" s="4"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34" s="29"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -3168,7 +3256,7 @@
       </c>
       <c r="F34" s="4"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35" s="29"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -3179,7 +3267,7 @@
       </c>
       <c r="F35" s="4"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" s="29"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -3190,7 +3278,7 @@
       </c>
       <c r="F36" s="4"/>
     </row>
-    <row r="37" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A37" s="30"/>
       <c r="B37" s="6"/>
       <c r="C37" s="6"/>
@@ -3199,7 +3287,7 @@
       </c>
       <c r="E37" s="26">
         <f>SUM(E3:E36)</f>
-        <v>6.25E-2</v>
+        <v>0.44166666666666676</v>
       </c>
       <c r="F37" s="7"/>
     </row>

</xml_diff>